<commit_message>
Optimizing Adding new plots
</commit_message>
<xml_diff>
--- a/Assignment_3/Results/halfkernel.xlsx
+++ b/Assignment_3/Results/halfkernel.xlsx
@@ -478,16 +478,16 @@
         <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>98.97</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
-        <v>99.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="F2" t="n">
         <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>99.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">

</xml_diff>